<commit_message>
Added boms for sun sense boards rev a
</commit_message>
<xml_diff>
--- a/eagle projects/Z- Sun Sensor Board/Z- Sun Sensor Board/BOM_Z-SUNSENSE.xlsx
+++ b/eagle projects/Z- Sun Sensor Board/Z- Sun Sensor Board/BOM_Z-SUNSENSE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Documents\EAGLE\projects\adcs_hardware\eagle projects\Z- Sun Sensor Board\Z- Sun Sensor Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3B56228-D92B-4036-9F8B-8324C3F1CC5F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF19811E-2712-419E-969C-AA22F75E9A45}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="1005" windowWidth="29040" windowHeight="15840" xr2:uid="{244178D5-7219-49F1-BCEF-521B6D6509EB}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="100">
   <si>
     <t>Value</t>
   </si>
@@ -199,9 +199,6 @@
     <t>REVISION: A</t>
   </si>
   <si>
-    <t>BOARD: Z- SUN SENSOR BOARD BILL OF  MATERIALS</t>
-  </si>
-  <si>
     <t>Item</t>
   </si>
   <si>
@@ -211,9 +208,6 @@
     <t>DO NOT POPULATE</t>
   </si>
   <si>
-    <t>Link</t>
-  </si>
-  <si>
     <t>Terminal Block Connector 1x02</t>
   </si>
   <si>
@@ -344,6 +338,18 @@
   </si>
   <si>
     <t>https://www.vishay.com/docs/45040/vj31vj34automlcc.pdf</t>
+  </si>
+  <si>
+    <t>BILL OF MATERIALS</t>
+  </si>
+  <si>
+    <t>Datasheet</t>
+  </si>
+  <si>
+    <t>Date: 2021.01.28</t>
+  </si>
+  <si>
+    <t>BOARD: Z- SUN SENSE BOARD</t>
   </si>
 </sst>
 </file>
@@ -541,7 +547,7 @@
     <tableColumn id="25" xr3:uid="{436F8E02-3893-44C1-A647-1B4DBD759357}" uniqueName="25" name="Footprint" queryTableFieldId="25" dataDxfId="1"/>
     <tableColumn id="27" xr3:uid="{6BD98B2B-A4F6-4353-A901-5BDD375D2756}" uniqueName="27" name="Description" queryTableFieldId="27"/>
     <tableColumn id="4" xr3:uid="{BE126D1A-8BE7-45C2-BDC5-337824793DF7}" uniqueName="4" name="Package" queryTableFieldId="4" dataDxfId="0"/>
-    <tableColumn id="7" xr3:uid="{91D1D211-2812-467E-AEFF-196F256AEC0A}" uniqueName="7" name="Link" queryTableFieldId="7" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{91D1D211-2812-467E-AEFF-196F256AEC0A}" uniqueName="7" name="Datasheet" queryTableFieldId="7" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -844,10 +850,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{929DA339-86DE-4673-A0B7-740D2A2A2D1A}">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -861,53 +867,54 @@
     <col min="7" max="7" width="27.21875" customWidth="1"/>
     <col min="8" max="8" width="61.77734375" style="8" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="24" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
       <c r="H1" s="7"/>
       <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-    </row>
-    <row r="2" spans="1:10" ht="25.8" x14ac:dyDescent="0.5">
+    </row>
+    <row r="2" spans="1:9" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A2" s="2" t="s">
-        <v>49</v>
+        <v>99</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="E2" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="F2" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G2" s="2"/>
+        <v>98</v>
+      </c>
+      <c r="G2" s="3"/>
       <c r="H2" s="7"/>
       <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>38</v>
@@ -922,7 +929,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>2</v>
@@ -931,10 +938,10 @@
         <v>1</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -942,36 +949,36 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5">
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>42</v>
@@ -980,56 +987,56 @@
         <v>8</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6">
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7">
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>44</v>
@@ -1038,94 +1045,94 @@
         <v>10</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8">
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9">
         <v>3</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G9" t="s">
         <v>52</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G9" t="s">
-        <v>54</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>15</v>
@@ -1134,18 +1141,18 @@
         <v>14</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11">
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>43</v>
@@ -1154,27 +1161,27 @@
         <v>16</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>18</v>
@@ -1183,27 +1190,27 @@
         <v>19</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>20</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>22</v>
@@ -1212,27 +1219,27 @@
         <v>23</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>24</v>
@@ -1241,27 +1248,27 @@
         <v>25</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>26</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15">
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>41</v>
@@ -1270,56 +1277,56 @@
         <v>21</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16">
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>45</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>27</v>
@@ -1328,10 +1335,10 @@
         <v>28</v>
       </c>
       <c r="F17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>29</v>
@@ -1342,13 +1349,13 @@
     </row>
     <row r="18" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>31</v>
@@ -1357,21 +1364,21 @@
         <v>32</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H18" s="9" t="s">
         <v>33</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19">
         <v>3</v>
@@ -1386,16 +1393,16 @@
         <v>34</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H19" s="9" t="s">
         <v>35</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>